<commit_message>
added lat/lon for lower Lemhi RST
</commit_message>
<xml_diff>
--- a/input/site/site_metadata.xlsx
+++ b/input/site/site_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PITcleanr_lite\inputs\site\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PITcleanr_lite\input\site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D1A7FD-5862-4D01-818E-2F7EA97EF9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE9C674-8A40-417B-854B-70086FD9F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3975" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,6 +187,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,11 +219,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +508,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +562,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>44.861600000000003</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>-113.63200000000001</v>
       </c>
       <c r="H2" t="b">
@@ -582,10 +586,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>44.866</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>-113.625</v>
       </c>
       <c r="H3" t="b">
@@ -608,10 +612,10 @@
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>44.874102000000001</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>-113.628846</v>
       </c>
       <c r="H4" t="b">
@@ -634,10 +638,10 @@
       <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>44.874225000000003</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>-113.628803</v>
       </c>
       <c r="H5" t="b">
@@ -660,10 +664,10 @@
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>44.876775000000002</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>-113.629752</v>
       </c>
       <c r="H6" t="b">
@@ -686,10 +690,10 @@
       <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>44.897005999999998</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>-113.625023</v>
       </c>
       <c r="H7" t="b">
@@ -712,10 +716,10 @@
       <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>44.897098999999997</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>-113.62515</v>
       </c>
       <c r="H8" t="b">
@@ -738,10 +742,10 @@
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>44.897393000000001</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>-113.624956</v>
       </c>
       <c r="H9" t="b">
@@ -764,10 +768,10 @@
       <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>44.897447</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>-113.62509300000001</v>
       </c>
       <c r="H10" t="b">
@@ -790,10 +794,10 @@
       <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>44.898980000000002</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>-113.626358</v>
       </c>
       <c r="H11" t="b">
@@ -816,10 +820,10 @@
       <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>44.899118999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>-113.626304</v>
       </c>
       <c r="H12" t="b">
@@ -842,10 +846,10 @@
       <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>44.899088999999996</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>-113.626735</v>
       </c>
       <c r="H13" t="b">
@@ -868,10 +872,10 @@
       <c r="E14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>44.899194999999999</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>-113.62661799999999</v>
       </c>
       <c r="H14" t="b">
@@ -894,10 +898,10 @@
       <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>44.899165000000004</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>-113.627179</v>
       </c>
       <c r="H15" t="b">
@@ -920,10 +924,10 @@
       <c r="E16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>44.899329999999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>-113.627334</v>
       </c>
       <c r="H16" t="b">
@@ -946,10 +950,10 @@
       <c r="E17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>44.899892000000001</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>-113.62796400000001</v>
       </c>
       <c r="H17" t="b">
@@ -972,10 +976,10 @@
       <c r="E18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>44.899987000000003</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>-113.62764199999999</v>
       </c>
       <c r="H18" t="b">
@@ -998,10 +1002,10 @@
       <c r="E19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>44.899906999999999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>-113.62769299999999</v>
       </c>
       <c r="H19" t="b">
@@ -1024,10 +1028,10 @@
       <c r="E20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>44.899949999999997</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>-113.62688300000001</v>
       </c>
       <c r="H20" t="b">
@@ -1050,10 +1054,10 @@
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>44.900218000000002</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>-113.62657400000001</v>
       </c>
       <c r="H21" t="b">
@@ -1074,10 +1078,10 @@
         <v>7</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>45.100099999999998</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>-113.726</v>
       </c>
       <c r="H22" t="b">
@@ -1097,10 +1101,10 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>45.109499999999997</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>-113.74299999999999</v>
       </c>
       <c r="H23" t="b">
@@ -1120,10 +1124,10 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>45.1113</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>-113.746</v>
       </c>
       <c r="H24" t="b">
@@ -1143,10 +1147,10 @@
       <c r="D25" t="s">
         <v>7</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>45.112200000000001</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>-113.747</v>
       </c>
       <c r="H25" t="b">
@@ -1166,10 +1170,10 @@
       <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>45.1128</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>-113.75</v>
       </c>
       <c r="H26" t="b">
@@ -1189,10 +1193,10 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>45.113199999999999</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>-113.756</v>
       </c>
       <c r="H27" t="b">
@@ -1212,10 +1216,10 @@
       <c r="D28" t="s">
         <v>7</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>45.115099999999998</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>-113.774</v>
       </c>
       <c r="H28" t="b">
@@ -1235,6 +1239,12 @@
       <c r="D29" t="s">
         <v>51</v>
       </c>
+      <c r="F29" s="2">
+        <v>45.159534999999998</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-113.833049</v>
+      </c>
       <c r="H29" t="b">
         <v>1</v>
       </c>
@@ -1252,10 +1262,10 @@
       <c r="D30" t="s">
         <v>7</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>45.176499999999997</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>-113.88500000000001</v>
       </c>
       <c r="H30" t="b">

</xml_diff>

<commit_message>
added reader info to site metadata
</commit_message>
<xml_diff>
--- a/input/site/site_metadata.xlsx
+++ b/input/site/site_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PITcleanr_lite\input\site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE9C674-8A40-417B-854B-70086FD9F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92983229-5ED6-4556-9094-153E41640296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="53">
   <si>
     <t>site_code</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>screw_trap</t>
+  </si>
+  <si>
+    <t>reader</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,12 +520,13 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,19 +540,22 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -561,18 +568,21 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2">
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2">
         <v>44.861600000000003</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>-113.63200000000001</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -585,18 +595,21 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2">
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2">
         <v>44.866</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>-113.625</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -609,20 +622,23 @@
       <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2">
         <v>44.874102000000001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>-113.628846</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -635,20 +651,23 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2">
         <v>44.874225000000003</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>-113.628803</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -661,20 +680,23 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2">
         <v>44.876775000000002</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>-113.629752</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -687,20 +709,23 @@
       <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2">
         <v>44.897005999999998</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>-113.625023</v>
       </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -713,20 +738,23 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
         <v>44.897098999999997</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-113.62515</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -739,20 +767,23 @@
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2">
         <v>44.897393000000001</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-113.624956</v>
       </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -765,20 +796,23 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2">
         <v>44.897447</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>-113.62509300000001</v>
       </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -791,20 +825,23 @@
       <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="E11" s="1">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2">
         <v>44.898980000000002</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>-113.626358</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -817,20 +854,23 @@
       <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="E12" s="1">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2">
         <v>44.899118999999999</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>-113.626304</v>
       </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -843,20 +883,23 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2">
         <v>44.899088999999996</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>-113.626735</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -869,20 +912,23 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2">
         <v>44.899194999999999</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>-113.62661799999999</v>
       </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -895,20 +941,23 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="1">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2">
         <v>44.899165000000004</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>-113.627179</v>
       </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -921,20 +970,23 @@
       <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="E16" s="1">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="2">
         <v>44.899329999999999</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>-113.627334</v>
       </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -947,20 +999,23 @@
       <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="E17" s="1">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2">
         <v>44.899892000000001</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>-113.62796400000001</v>
       </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -973,20 +1028,23 @@
       <c r="D18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="E18" s="1">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2">
         <v>44.899987000000003</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>-113.62764199999999</v>
       </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -999,20 +1057,23 @@
       <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="E19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2">
         <v>44.899906999999999</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>-113.62769299999999</v>
       </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1025,20 +1086,23 @@
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20" s="1">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2">
         <v>44.899949999999997</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>-113.62688300000001</v>
       </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1051,20 +1115,23 @@
       <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E21" s="1">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2">
         <v>44.900218000000002</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>-113.62657400000001</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1077,18 +1144,21 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2">
+      <c r="E22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2">
         <v>45.100099999999998</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>-113.726</v>
       </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1101,17 +1171,20 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2">
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2">
         <v>45.109499999999997</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>-113.74299999999999</v>
       </c>
-      <c r="H23" t="b">
+      <c r="I23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1124,17 +1197,20 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="2">
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="2">
         <v>45.1113</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>-113.746</v>
       </c>
-      <c r="H24" t="b">
+      <c r="I24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1147,17 +1223,20 @@
       <c r="D25" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="2">
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="2">
         <v>45.112200000000001</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>-113.747</v>
       </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1170,17 +1249,20 @@
       <c r="D26" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="2">
+      <c r="E26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2">
         <v>45.1128</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>-113.75</v>
       </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1193,17 +1275,20 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="2">
+      <c r="E27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="2">
         <v>45.113199999999999</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>-113.756</v>
       </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1216,17 +1301,20 @@
       <c r="D28" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="2">
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="2">
         <v>45.115099999999998</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>-113.774</v>
       </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1239,17 +1327,20 @@
       <c r="D29" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="2">
+      <c r="E29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="2">
         <v>45.159534999999998</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>-113.833049</v>
       </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1262,13 +1353,16 @@
       <c r="D30" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="2">
+      <c r="E30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="2">
         <v>45.176499999999997</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>-113.88500000000001</v>
       </c>
-      <c r="H30" t="b">
+      <c r="I30" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>